<commit_message>
Thiet ke CSDL, TKTT, lua chong cong nghe
</commit_message>
<xml_diff>
--- a/ThietkeCSDL.xlsx
+++ b/ThietkeCSDL.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="MotaTongquan" sheetId="3" r:id="rId1"/>
-    <sheet name="ModuleQLND" sheetId="1" r:id="rId2"/>
-    <sheet name="QuanlyCauhoi" sheetId="2" r:id="rId3"/>
-    <sheet name="Quản lý tiền và giao dịch" sheetId="4" r:id="rId4"/>
+    <sheet name="ModuleQLND" sheetId="1" r:id="rId1"/>
+    <sheet name="QuanlyCauhoi" sheetId="2" r:id="rId2"/>
+    <sheet name="Quản lý tiền và giao dịch" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="84">
   <si>
     <t>1. USER</t>
   </si>
@@ -216,6 +215,64 @@
   </si>
   <si>
     <t>Quản lý nạp tiền</t>
+  </si>
+  <si>
+    <t>money_deposit_id</t>
+  </si>
+  <si>
+    <t>deposit_date</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>number(2)</t>
+  </si>
+  <si>
+    <t>- nạp thẻ điện thoại
+- nạp thẻ thanh toán quốc tế</t>
+  </si>
+  <si>
+    <t>deposit_money</t>
+  </si>
+  <si>
+    <t>actual_point</t>
+  </si>
+  <si>
+    <t>2. TRANSACTION</t>
+  </si>
+  <si>
+    <t>transaction_id</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Loại giao dịch: 
+1. chơi cá độ
+2. thắng tiền cá độ
+3. chuyển tiền</t>
+  </si>
+  <si>
+    <t>user_create_id</t>
+  </si>
+  <si>
+    <t>from_user_id</t>
+  </si>
+  <si>
+    <t>to_user_id</t>
+  </si>
+  <si>
+    <t>nếu chuyển tiền thuộc loại 1 và 2 thì lưu id câu hỏi</t>
+  </si>
+  <si>
+    <t>total_point</t>
+  </si>
+  <si>
+    <t>total_deposit_money</t>
   </si>
 </sst>
 </file>
@@ -279,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -296,9 +353,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -306,6 +360,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,24 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,12 +693,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -786,130 +841,160 @@
       </c>
       <c r="F16" s="2"/>
     </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="6">
+        <v>11</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="6">
+        <v>12</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="3" t="s">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="6">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="6">
-        <v>2</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="E24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="6">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="6">
-        <v>3</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="6">
+        <v>3</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="7" t="s">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D27" s="1" t="s">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D28" s="1" t="s">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" s="3" t="s">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="6">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2" t="s">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="6">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="6">
-        <v>2</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="E36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="6">
+        <v>2</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="6">
-        <v>3</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="E37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C38" s="6">
+        <v>3</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -920,11 +1005,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -939,12 +1024,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -1017,10 +1102,10 @@
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -1148,7 +1233,7 @@
       <c r="E26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="8" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1174,7 +1259,7 @@
       <c r="E28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1360,7 +1445,7 @@
       <c r="E48" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="F48" s="8" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1386,7 +1471,7 @@
       <c r="E50" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1446,7 +1531,7 @@
       <c r="E58" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F58" s="9"/>
+      <c r="F58" s="8"/>
     </row>
     <row r="59" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C59" s="6">
@@ -1458,7 +1543,7 @@
       <c r="E59" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F59" s="9" t="s">
+      <c r="F59" s="8" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1472,7 +1557,7 @@
       <c r="E60" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F60" s="9" t="s">
+      <c r="F60" s="8" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1484,12 +1569,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F35"/>
+  <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,12 +1588,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -1537,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
@@ -1549,10 +1634,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -1561,10 +1646,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -1573,211 +1658,145 @@
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C11" s="6">
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" s="6">
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="13">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="13">
+        <v>2</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="13">
+        <v>3</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C20" s="13">
+        <v>4</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="13">
+        <v>5</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="13">
+        <v>6</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C23" s="13">
         <v>7</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="6">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="6">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="6">
-        <v>9</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="6">
-        <v>10</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="6">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="6">
-        <v>2</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="6">
-        <v>3</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D27" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D28" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="6">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="6">
-        <v>2</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="6">
-        <v>3</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" s="2"/>
+      <c r="D23" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>